<commit_message>
ler planilha e iterar por cada linha
</commit_message>
<xml_diff>
--- a/clientes.xlsx
+++ b/clientes.xlsx
@@ -13,6 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
+    <sheet name="Planilha3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -448,4 +450,30 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
formatar mensagem e abrir link de envio no navegador
</commit_message>
<xml_diff>
--- a/clientes.xlsx
+++ b/clientes.xlsx
@@ -85,9 +85,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,7 +372,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B2" sqref="B2:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -396,8 +397,8 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
-        <v>12345678912</v>
+      <c r="B2" s="2">
+        <v>5581945678912</v>
       </c>
       <c r="C2" s="1">
         <v>45706</v>
@@ -407,8 +408,8 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
-        <v>12345678912</v>
+      <c r="B3" s="2">
+        <v>5581945678912</v>
       </c>
       <c r="C3" s="1">
         <v>45706</v>
@@ -418,8 +419,8 @@
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
-        <v>12345678912</v>
+      <c r="B4" s="2">
+        <v>5581945678912</v>
       </c>
       <c r="C4" s="1">
         <v>45706</v>
@@ -429,8 +430,8 @@
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5">
-        <v>12345678912</v>
+      <c r="B5" s="2">
+        <v>5581945678912</v>
       </c>
       <c r="C5" s="1">
         <v>45706</v>
@@ -440,8 +441,8 @@
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6">
-        <v>12345678912</v>
+      <c r="B6" s="2">
+        <v>5581945678912</v>
       </c>
       <c r="C6" s="1">
         <v>45706</v>

</xml_diff>